<commit_message>
[docs] Updated static_analysis_20210616_V1.1.0.xlsx and phase1_document_team6.xlsx
static_analysis_20210616_V1.1.0.xlsx and phase1_document_team6.xlsx
</commit_message>
<xml_diff>
--- a/docs/09_static_analysis/static_analysis_20210616_v1.1.0_reviewed.xlsx
+++ b/docs/09_static_analysis/static_analysis_20210616_v1.1.0_reviewed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cppchecker_20210616_v1.1.0" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'cppchecker_20210616_v1.1.0'!$C$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">flawfinder_20210616_v1.1.0!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">flawfinder_20210616_v1.1.0!$D$4:$E$109</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="113">
   <si>
     <t>File</t>
   </si>
@@ -335,24 +335,52 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>be careful</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condition 'argc==3' is always false</t>
+  </si>
+  <si>
+    <t>Variable 'op_type' is assigned in constructor body. Consider performing initialization in initialization list.</t>
+  </si>
+  <si>
+    <t>temp\cmu_project\source\common\Logger.cpp</t>
+  </si>
+  <si>
+    <t>The function 'log_hexdump' is never used.</t>
+  </si>
+  <si>
     <t>close</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>be careful</t>
+    <t>fix</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Condition 'argc==3' is always false</t>
-  </si>
-  <si>
-    <t>Variable 'op_type' is assigned in constructor body. Consider performing initialization in initialization list.</t>
-  </si>
-  <si>
-    <t>temp\cmu_project\source\common\Logger.cpp</t>
-  </si>
-  <si>
-    <t>The function 'log_hexdump' is never used.</t>
+    <t>close</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>not a bug</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>open</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>add exception</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>add exception</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>check strlen</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2385,7 +2413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -2428,7 +2456,7 @@
         <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2666,7 +2694,7 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2977,7 +3005,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B35">
         <v>124</v>
@@ -2989,7 +3017,7 @@
         <v>6</v>
       </c>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3003,10 +3031,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:I113"/>
+  <dimension ref="A4:I109"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3037,11 +3065,11 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
         <v>100</v>
-      </c>
-      <c r="E7" t="s">
-        <v>101</v>
       </c>
       <c r="F7" t="s">
         <v>99</v>
@@ -3061,6 +3089,12 @@
       <c r="B10">
         <v>2</v>
       </c>
+      <c r="D10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
       <c r="F10" t="s">
         <v>77</v>
       </c>
@@ -3079,6 +3113,12 @@
       <c r="B13">
         <v>3</v>
       </c>
+      <c r="D13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" t="s">
+        <v>100</v>
+      </c>
       <c r="F13" t="s">
         <v>78</v>
       </c>
@@ -3097,6 +3137,12 @@
       <c r="B16">
         <v>4</v>
       </c>
+      <c r="D16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" t="s">
+        <v>106</v>
+      </c>
       <c r="F16" t="s">
         <v>79</v>
       </c>
@@ -3125,6 +3171,12 @@
       <c r="B21">
         <v>5</v>
       </c>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" t="s">
+        <v>106</v>
+      </c>
       <c r="F21" t="s">
         <v>80</v>
       </c>
@@ -3153,6 +3205,12 @@
       <c r="B26">
         <v>6</v>
       </c>
+      <c r="D26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" t="s">
+        <v>100</v>
+      </c>
       <c r="F26" t="s">
         <v>81</v>
       </c>
@@ -3171,6 +3229,12 @@
       <c r="B29">
         <v>7</v>
       </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
+        <v>100</v>
+      </c>
       <c r="F29" t="s">
         <v>82</v>
       </c>
@@ -3189,6 +3253,12 @@
       <c r="B32">
         <v>8</v>
       </c>
+      <c r="D32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" t="s">
+        <v>106</v>
+      </c>
       <c r="F32" t="s">
         <v>83</v>
       </c>
@@ -3217,6 +3287,12 @@
       <c r="B37">
         <v>9</v>
       </c>
+      <c r="D37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" t="s">
+        <v>106</v>
+      </c>
       <c r="F37" t="s">
         <v>84</v>
       </c>
@@ -3245,6 +3321,12 @@
       <c r="B42">
         <v>10</v>
       </c>
+      <c r="D42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" t="s">
+        <v>108</v>
+      </c>
       <c r="F42" t="s">
         <v>85</v>
       </c>
@@ -3263,6 +3345,12 @@
       <c r="B45">
         <v>11</v>
       </c>
+      <c r="D45" t="s">
+        <v>107</v>
+      </c>
+      <c r="E45" t="s">
+        <v>108</v>
+      </c>
       <c r="F45" t="s">
         <v>63</v>
       </c>
@@ -3281,6 +3369,12 @@
       <c r="B48">
         <v>12</v>
       </c>
+      <c r="D48" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48" t="s">
+        <v>108</v>
+      </c>
       <c r="F48" t="s">
         <v>86</v>
       </c>
@@ -3299,6 +3393,12 @@
       <c r="B51">
         <v>13</v>
       </c>
+      <c r="D51" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" t="s">
+        <v>108</v>
+      </c>
       <c r="F51" t="s">
         <v>64</v>
       </c>
@@ -3317,6 +3417,12 @@
       <c r="B54">
         <v>14</v>
       </c>
+      <c r="D54" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" t="s">
+        <v>108</v>
+      </c>
       <c r="F54" t="s">
         <v>87</v>
       </c>
@@ -3335,6 +3441,12 @@
       <c r="B57">
         <v>15</v>
       </c>
+      <c r="D57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" t="s">
+        <v>110</v>
+      </c>
       <c r="F57" t="s">
         <v>88</v>
       </c>
@@ -3353,6 +3465,12 @@
       <c r="B60">
         <v>16</v>
       </c>
+      <c r="D60" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" t="s">
+        <v>111</v>
+      </c>
       <c r="F60" t="s">
         <v>89</v>
       </c>
@@ -3371,6 +3489,12 @@
       <c r="B63">
         <v>17</v>
       </c>
+      <c r="D63" t="s">
+        <v>109</v>
+      </c>
+      <c r="E63" t="s">
+        <v>112</v>
+      </c>
       <c r="F63" t="s">
         <v>90</v>
       </c>
@@ -3389,6 +3513,12 @@
       <c r="B66">
         <v>18</v>
       </c>
+      <c r="D66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E66" t="s">
+        <v>112</v>
+      </c>
       <c r="F66" t="s">
         <v>90</v>
       </c>
@@ -3407,6 +3537,12 @@
       <c r="B69">
         <v>19</v>
       </c>
+      <c r="D69" t="s">
+        <v>109</v>
+      </c>
+      <c r="E69" t="s">
+        <v>110</v>
+      </c>
       <c r="F69" t="s">
         <v>91</v>
       </c>
@@ -3425,6 +3561,12 @@
       <c r="B72">
         <v>20</v>
       </c>
+      <c r="D72" t="s">
+        <v>109</v>
+      </c>
+      <c r="E72" t="s">
+        <v>110</v>
+      </c>
       <c r="F72" t="s">
         <v>92</v>
       </c>
@@ -3443,6 +3585,12 @@
       <c r="B75">
         <v>21</v>
       </c>
+      <c r="D75" t="s">
+        <v>109</v>
+      </c>
+      <c r="E75" t="s">
+        <v>110</v>
+      </c>
       <c r="F75" t="s">
         <v>93</v>
       </c>
@@ -3461,6 +3609,12 @@
       <c r="B78">
         <v>22</v>
       </c>
+      <c r="D78" t="s">
+        <v>109</v>
+      </c>
+      <c r="E78" t="s">
+        <v>112</v>
+      </c>
       <c r="F78" t="s">
         <v>94</v>
       </c>
@@ -3479,6 +3633,12 @@
       <c r="B81">
         <v>23</v>
       </c>
+      <c r="D81" t="s">
+        <v>109</v>
+      </c>
+      <c r="E81" t="s">
+        <v>112</v>
+      </c>
       <c r="F81" t="s">
         <v>95</v>
       </c>
@@ -3497,6 +3657,12 @@
       <c r="B84">
         <v>24</v>
       </c>
+      <c r="D84" t="s">
+        <v>107</v>
+      </c>
+      <c r="E84" t="s">
+        <v>108</v>
+      </c>
       <c r="F84" t="s">
         <v>65</v>
       </c>
@@ -3515,6 +3681,12 @@
       <c r="B87">
         <v>25</v>
       </c>
+      <c r="D87" t="s">
+        <v>107</v>
+      </c>
+      <c r="E87" t="s">
+        <v>108</v>
+      </c>
       <c r="F87" t="s">
         <v>66</v>
       </c>
@@ -3533,6 +3705,12 @@
       <c r="B90">
         <v>26</v>
       </c>
+      <c r="D90" t="s">
+        <v>107</v>
+      </c>
+      <c r="E90" t="s">
+        <v>108</v>
+      </c>
       <c r="F90" t="s">
         <v>67</v>
       </c>
@@ -3551,6 +3729,12 @@
       <c r="B93">
         <v>27</v>
       </c>
+      <c r="D93" t="s">
+        <v>107</v>
+      </c>
+      <c r="E93" t="s">
+        <v>108</v>
+      </c>
       <c r="F93" t="s">
         <v>68</v>
       </c>
@@ -3569,6 +3753,12 @@
       <c r="B96">
         <v>28</v>
       </c>
+      <c r="D96" t="s">
+        <v>107</v>
+      </c>
+      <c r="E96" t="s">
+        <v>108</v>
+      </c>
       <c r="F96" t="s">
         <v>96</v>
       </c>
@@ -3587,6 +3777,12 @@
       <c r="B99">
         <v>29</v>
       </c>
+      <c r="D99" t="s">
+        <v>107</v>
+      </c>
+      <c r="E99" t="s">
+        <v>108</v>
+      </c>
       <c r="F99" t="s">
         <v>97</v>
       </c>
@@ -3605,6 +3801,12 @@
       <c r="B102">
         <v>30</v>
       </c>
+      <c r="D102" t="s">
+        <v>107</v>
+      </c>
+      <c r="E102" t="s">
+        <v>108</v>
+      </c>
       <c r="F102" t="s">
         <v>98</v>
       </c>
@@ -3619,26 +3821,33 @@
         <v>50</v>
       </c>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F112" t="s">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F108" t="s">
         <v>72</v>
       </c>
-      <c r="G112" t="s">
+      <c r="G108" t="s">
         <v>73</v>
       </c>
-      <c r="H112" t="s">
+      <c r="H108" t="s">
         <v>74</v>
       </c>
-      <c r="I112" t="s">
+      <c r="I108" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="113" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F113">
-        <v>36</v>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F109">
+        <v>30</v>
+      </c>
+      <c r="G109">
+        <v>9</v>
+      </c>
+      <c r="H109">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D4:E109"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>